<commit_message>
Single cycle datapath + controlpath completes here. The next step is to implement a pipelined flow in the processor.
</commit_message>
<xml_diff>
--- a/ControlWordsGenerator/InsWordParams.xlsx
+++ b/ControlWordsGenerator/InsWordParams.xlsx
@@ -189,6 +189,21 @@
     <t>L</t>
   </si>
   <si>
+    <t>A + C'D + B'C</t>
+  </si>
+  <si>
+    <t>B'D + B'C + BD'</t>
+  </si>
+  <si>
+    <t>B'C + CD + AD + BC'D'</t>
+  </si>
+  <si>
+    <t>C'D + B'C</t>
+  </si>
+  <si>
+    <t>CD' + BD' + B'D</t>
+  </si>
+  <si>
     <r>
       <t>A</t>
     </r>
@@ -205,28 +220,13 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>B'</t>
     </r>
-  </si>
-  <si>
-    <t>A + C'D + B'C</t>
-  </si>
-  <si>
-    <t>B'D + B'C + BD'</t>
-  </si>
-  <si>
-    <t>B'C + CD + AD + BC'D'</t>
-  </si>
-  <si>
-    <t>C'D + B'C</t>
-  </si>
-  <si>
-    <t>CD' + BD' + B'D</t>
   </si>
 </sst>
 </file>
@@ -258,14 +258,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1" tint="0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1" tint="0.34998626667073579"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -370,14 +370,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,9 +694,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AG37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA21" sqref="AA21:AD21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +709,7 @@
     <col min="6" max="6" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="1"/>
     <col min="8" max="8" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" style="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -881,15 +881,15 @@
       <c r="AD2" s="4">
         <v>0</v>
       </c>
-      <c r="AE2" s="15">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="14" t="s">
-        <v>54</v>
+      <c r="AE2" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B3" s="10"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
@@ -968,15 +968,15 @@
       <c r="AD3" s="4">
         <v>0</v>
       </c>
-      <c r="AE3" s="15">
-        <v>1</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>55</v>
+      <c r="AE3" s="10">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B4" s="10"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1055,15 +1055,15 @@
       <c r="AD4" s="4">
         <v>1</v>
       </c>
-      <c r="AE4" s="15">
+      <c r="AE4" s="10">
         <v>2</v>
       </c>
-      <c r="AG4" t="s">
-        <v>56</v>
+      <c r="AG4" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1131,15 +1131,15 @@
         <v>1</v>
       </c>
       <c r="AD5" s="4"/>
-      <c r="AE5" s="15">
+      <c r="AE5" s="10">
         <v>3</v>
       </c>
-      <c r="AG5" t="s">
-        <v>57</v>
+      <c r="AG5" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1218,12 +1218,12 @@
       <c r="AD6" s="4">
         <v>1</v>
       </c>
-      <c r="AE6" s="15">
+      <c r="AE6" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="1" t="s">
         <v>38</v>
       </c>
@@ -1302,12 +1302,12 @@
       <c r="AD7" s="4">
         <v>0</v>
       </c>
-      <c r="AE7" s="15">
+      <c r="AE7" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
         <v>39</v>
       </c>
@@ -1386,12 +1386,12 @@
       <c r="AD8" s="4">
         <v>0</v>
       </c>
-      <c r="AE8" s="15">
+      <c r="AE8" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="1" t="s">
         <v>40</v>
       </c>
@@ -1470,12 +1470,12 @@
       <c r="AD9" s="4">
         <v>1</v>
       </c>
-      <c r="AE9" s="15">
+      <c r="AE9" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="1" t="s">
         <v>41</v>
       </c>
@@ -1554,12 +1554,12 @@
       <c r="AD10" s="4">
         <v>0</v>
       </c>
-      <c r="AE10" s="15">
+      <c r="AE10" s="10">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
+      <c r="B11" s="12"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1594,12 +1594,12 @@
         <v>1</v>
       </c>
       <c r="AD11" s="4"/>
-      <c r="AE11" s="15">
+      <c r="AE11" s="10">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="1" t="s">
         <v>43</v>
       </c>
@@ -1667,12 +1667,12 @@
         <v>0</v>
       </c>
       <c r="AD12" s="4"/>
-      <c r="AE12" s="15">
+      <c r="AE12" s="10">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
+      <c r="B13" s="12"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1707,12 +1707,12 @@
         <v>1</v>
       </c>
       <c r="AD13" s="4"/>
-      <c r="AE13" s="15">
+      <c r="AE13" s="10">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1780,12 +1780,12 @@
         <v>0</v>
       </c>
       <c r="AD14" s="4"/>
-      <c r="AE14" s="15">
+      <c r="AE14" s="10">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1864,12 +1864,12 @@
       <c r="AD15" s="4">
         <v>1</v>
       </c>
-      <c r="AE15" s="15">
+      <c r="AE15" s="10">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1931,12 +1931,12 @@
         <v>0</v>
       </c>
       <c r="AD16" s="4"/>
-      <c r="AE16" s="15">
+      <c r="AE16" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1998,12 +1998,12 @@
         <v>1</v>
       </c>
       <c r="AD17" s="4"/>
-      <c r="AE17" s="15">
+      <c r="AE17" s="10">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="1" t="s">
         <v>27</v>
       </c>
@@ -2054,7 +2054,7 @@
       </c>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="1" t="s">
         <v>28</v>
       </c>
@@ -2105,7 +2105,7 @@
       </c>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="1" t="s">
         <v>29</v>
       </c>
@@ -2156,7 +2156,7 @@
       </c>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="1" t="s">
         <v>26</v>
       </c>
@@ -2221,7 +2221,7 @@
       <c r="AD21" s="6"/>
     </row>
     <row r="22" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="1" t="s">
         <v>25</v>
       </c>
@@ -2297,7 +2297,7 @@
       <c r="AD22" s="4">
         <v>0</v>
       </c>
-      <c r="AE22" s="15">
+      <c r="AE22" s="10">
         <v>0</v>
       </c>
       <c r="AG22" s="1">
@@ -2305,7 +2305,7 @@
       </c>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
+      <c r="B23" s="13"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -2345,15 +2345,15 @@
       <c r="AD23" s="4">
         <v>0</v>
       </c>
-      <c r="AE23" s="15">
-        <v>1</v>
-      </c>
-      <c r="AG23" t="s">
-        <v>58</v>
+      <c r="AE23" s="10">
+        <v>1</v>
+      </c>
+      <c r="AG23" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="1" t="s">
         <v>46</v>
       </c>
@@ -2426,15 +2426,15 @@
       <c r="AD24" s="4">
         <v>1</v>
       </c>
-      <c r="AE24" s="15">
+      <c r="AE24" s="10">
         <v>2</v>
       </c>
-      <c r="AG24" t="s">
-        <v>59</v>
+      <c r="AG24" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="1" t="s">
         <v>46</v>
       </c>
@@ -2496,15 +2496,15 @@
         <v>1</v>
       </c>
       <c r="AD25" s="4"/>
-      <c r="AE25" s="15">
+      <c r="AE25" s="10">
         <v>3</v>
       </c>
-      <c r="AG25" t="s">
-        <v>57</v>
+      <c r="AG25" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="1" t="s">
         <v>47</v>
       </c>
@@ -2577,12 +2577,12 @@
       <c r="AD26" s="4">
         <v>1</v>
       </c>
-      <c r="AE26" s="15">
+      <c r="AE26" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B27" s="11"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="1" t="s">
         <v>47</v>
       </c>
@@ -2655,12 +2655,12 @@
       <c r="AD27" s="4">
         <v>0</v>
       </c>
-      <c r="AE27" s="15">
+      <c r="AE27" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="1" t="s">
         <v>48</v>
       </c>
@@ -2733,12 +2733,12 @@
       <c r="AD28" s="4">
         <v>0</v>
       </c>
-      <c r="AE28" s="15">
+      <c r="AE28" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B29" s="11"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
@@ -2811,12 +2811,12 @@
       <c r="AD29" s="4">
         <v>1</v>
       </c>
-      <c r="AE29" s="15">
+      <c r="AE29" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B30" s="11"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="1" t="s">
         <v>49</v>
       </c>
@@ -2889,12 +2889,12 @@
       <c r="AD30" s="4">
         <v>0</v>
       </c>
-      <c r="AE30" s="15">
+      <c r="AE30" s="10">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B31" s="11"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="1" t="s">
         <v>49</v>
       </c>
@@ -2956,12 +2956,12 @@
         <v>1</v>
       </c>
       <c r="AD31" s="4"/>
-      <c r="AE31" s="15">
+      <c r="AE31" s="10">
         <v>9</v>
       </c>
     </row>
     <row r="32" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B32" s="11"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="1" t="s">
         <v>49</v>
       </c>
@@ -3034,12 +3034,12 @@
       <c r="AD32" s="4">
         <v>1</v>
       </c>
-      <c r="AE32" s="15">
+      <c r="AE32" s="10">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B33" s="11"/>
+      <c r="B33" s="13"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -3068,12 +3068,12 @@
         <v>1</v>
       </c>
       <c r="AD33" s="4"/>
-      <c r="AE33" s="15">
+      <c r="AE33" s="10">
         <v>11</v>
       </c>
     </row>
     <row r="34" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="12"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="1" t="s">
         <v>52</v>
       </c>
@@ -3146,7 +3146,7 @@
       <c r="AD34" s="4">
         <v>1</v>
       </c>
-      <c r="AE34" s="15">
+      <c r="AE34" s="10">
         <v>12</v>
       </c>
     </row>
@@ -3175,7 +3175,7 @@
       <c r="AD35" s="4">
         <v>1</v>
       </c>
-      <c r="AE35" s="15">
+      <c r="AE35" s="10">
         <v>13</v>
       </c>
     </row>
@@ -3204,7 +3204,7 @@
       <c r="AD36" s="4">
         <v>0</v>
       </c>
-      <c r="AE36" s="15">
+      <c r="AE36" s="10">
         <v>14</v>
       </c>
     </row>
@@ -3233,7 +3233,7 @@
       <c r="AD37" s="4">
         <v>1</v>
       </c>
-      <c r="AE37" s="15">
+      <c r="AE37" s="10">
         <v>15</v>
       </c>
     </row>

</xml_diff>